<commit_message>
Dodan mikrokontroler komponenta u listu materijala.
</commit_message>
<xml_diff>
--- a/pcb_design/kicad_schematics/materials list/tabela sa komponentama_1.xlsx
+++ b/pcb_design/kicad_schematics/materials list/tabela sa komponentama_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Desktop\ETF\IV\MIKROKONTROLERI\ColorSorter_A\pcb_design\kicad_schematics\materials list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C52B006-024C-4486-8436-01FCC74F4A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C655572-A76A-4D05-8BF9-B4131F0F0927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Naziv komponente</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>UKUPNO</t>
+  </si>
+  <si>
+    <t>PIC24FJ64GA702-I/SO</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>579-24FJ64GA702ISO</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#.##0\ [$€-1];[Red]\-#.##0\ [$€-1]"/>
+    <numFmt numFmtId="164" formatCode="#.##0\ [$€-1];[Red]\-#.##0\ [$€-1]"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -310,9 +319,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -320,21 +329,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="medium">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="medium">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -349,26 +377,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="medium">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="medium">
-          <color auto="1"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -519,17 +527,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{476FECB3-D02A-40AC-8DE7-491427D36F7C}" name="Table1" displayName="Table1" ref="C4:H17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="C4:H17" xr:uid="{476FECB3-D02A-40AC-8DE7-491427D36F7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{476FECB3-D02A-40AC-8DE7-491427D36F7C}" name="Table1" displayName="Table1" ref="C4:H18" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="C4:H18" xr:uid="{476FECB3-D02A-40AC-8DE7-491427D36F7C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9C4880AB-57D2-4A43-A39B-D946936C8661}" name="Naziv komponente" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FFB753FB-35A8-4BD9-B4EA-5ED17045BD80}" name="Količina" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{7A770332-0DD7-4B5A-B095-F3CE31EE4B29}" name="Vrijednost" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{B3575CCB-DDA2-42E5-A79E-E98AA3ED03D4}" name="Cijena po komadu" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{20409220-FCA9-494E-ACD3-EA22BE4B0E8D}" name="Cijena po količini" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{20409220-FCA9-494E-ACD3-EA22BE4B0E8D}" name="Cijena po količini" dataDxfId="1">
       <calculatedColumnFormula xml:space="preserve"> D5*Table1[[#This Row],[Cijena po komadu]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DB2D81C7-1EDC-40B1-8BE9-8928F3046521}" name="Šifra (Mouser Part No)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DB2D81C7-1EDC-40B1-8BE9-8928F3046521}" name="Šifra (Mouser Part No)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -798,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:H22"/>
+  <dimension ref="C4:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,10 +851,10 @@
       <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="6">
         <v>0.152</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="7">
         <f xml:space="preserve"> D5*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>1.0640000000000001</v>
       </c>
@@ -864,10 +872,10 @@
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="7">
         <f xml:space="preserve"> D6*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.66500000000000004</v>
       </c>
@@ -885,14 +893,14 @@
       <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>0.627</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <f xml:space="preserve"> D7*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>1.881</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -906,14 +914,14 @@
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>0.18099999999999999</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <f xml:space="preserve"> D8*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.54299999999999993</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -927,10 +935,10 @@
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="7">
         <f xml:space="preserve"> D9*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.28500000000000003</v>
       </c>
@@ -948,10 +956,10 @@
       <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="7">
         <f xml:space="preserve"> D10*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.19</v>
       </c>
@@ -969,10 +977,10 @@
       <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="7">
         <f xml:space="preserve"> D11*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.19</v>
       </c>
@@ -990,10 +998,10 @@
       <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="6">
         <v>0.19</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="7">
         <f xml:space="preserve"> D12*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.38</v>
       </c>
@@ -1011,10 +1019,10 @@
       <c r="E13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="6">
         <v>0.14299999999999999</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="7">
         <f xml:space="preserve"> D13*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.14299999999999999</v>
       </c>
@@ -1032,10 +1040,10 @@
       <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="6">
         <v>0.219</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="7">
         <f xml:space="preserve"> D14*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>0.65700000000000003</v>
       </c>
@@ -1053,10 +1061,10 @@
       <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="6">
         <v>0.58899999999999997</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="7">
         <f xml:space="preserve"> D15*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>1.1779999999999999</v>
       </c>
@@ -1074,10 +1082,10 @@
       <c r="E16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="6">
         <v>1.61</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="7">
         <f xml:space="preserve"> D16*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>3.22</v>
       </c>
@@ -1085,28 +1093,49 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="16" t="s">
+    <row r="17" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="G17" s="16">
+        <f xml:space="preserve"> Table1[[#This Row],[Količina]]*Table1[[#This Row],[Cijena po komadu]]</f>
+        <v>3.34</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="8">
-        <f>SUM(D5:D16)</f>
-        <v>37</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9">
-        <f>SUM(F5:F16)</f>
-        <v>4.0910000000000002</v>
-      </c>
-      <c r="G17" s="15">
-        <f xml:space="preserve"> SUM(G5:G16)</f>
-        <v>10.396000000000001</v>
-      </c>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="D18" s="8">
+        <f>SUM(D5:D17)</f>
+        <v>39</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9">
+        <f>SUM(F5:F17)</f>
+        <v>5.7610000000000001</v>
+      </c>
+      <c r="G18" s="13">
+        <f xml:space="preserve"> SUM(G5:G17)</f>
+        <v>13.736000000000001</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Dodani u inc.h potrebni define
</commit_message>
<xml_diff>
--- a/pcb_design/kicad_schematics/materials list/tabela sa komponentama_1.xlsx
+++ b/pcb_design/kicad_schematics/materials list/tabela sa komponentama_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Desktop\ETF\IV\MIKROKONTROLERI\ColorSorter_A\pcb_design\kicad_schematics\materials list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C655572-A76A-4D05-8BF9-B4131F0F0927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134F0FE-A8CE-4B7E-A615-FCE39DE63AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -336,7 +336,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,7 +1105,7 @@
       <c r="F17" s="6">
         <v>1.67</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="7">
         <f xml:space="preserve"> Table1[[#This Row],[Količina]]*Table1[[#This Row],[Cijena po komadu]]</f>
         <v>3.34</v>
       </c>

</xml_diff>